<commit_message>
updated sprint spreadsheet for week 2
</commit_message>
<xml_diff>
--- a/Documentation/Sprint Planning/Planning - NaaiTek.xlsx
+++ b/Documentation/Sprint Planning/Planning - NaaiTek.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4660" yWindow="2220" windowWidth="25600" windowHeight="14640" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Description and Releases" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="58">
   <si>
     <t>ISSUE</t>
   </si>
@@ -173,6 +173,57 @@
   </si>
   <si>
     <t>Setup basic Prolog webservice</t>
+  </si>
+  <si>
+    <t>Setup basic JSON parser in C++</t>
+  </si>
+  <si>
+    <t>AS, AT</t>
+  </si>
+  <si>
+    <t>Improve graph search algorithms</t>
+  </si>
+  <si>
+    <t>Improve Prolog webservice</t>
+  </si>
+  <si>
+    <t>Implement AI ("CRUD" on knowledge base)</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>Enable authentication and roles</t>
+  </si>
+  <si>
+    <t>Create bootstrap for website</t>
+  </si>
+  <si>
+    <t>Enable globalization (language-wise)</t>
+  </si>
+  <si>
+    <t>AT</t>
+  </si>
+  <si>
+    <t>Minigame: tic-tac-toe</t>
+  </si>
+  <si>
+    <t>Minigame: labyrinth</t>
+  </si>
+  <si>
+    <t>Minigame: hangman</t>
+  </si>
+  <si>
+    <t>Create login to 3D</t>
+  </si>
+  <si>
+    <t>Improve graph design</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>JC</t>
   </si>
 </sst>
 </file>
@@ -444,8 +495,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -509,9 +564,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -576,10 +628,17 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -884,7 +943,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M35"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
       <selection activeCell="S31" sqref="S31"/>
     </sheetView>
   </sheetViews>
@@ -913,90 +972,90 @@
       <c r="M2" s="3"/>
     </row>
     <row r="3" spans="2:13">
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="42"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="41"/>
     </row>
     <row r="4" spans="2:13">
-      <c r="B4" s="43"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="44"/>
-      <c r="M4" s="45"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="44"/>
     </row>
     <row r="5" spans="2:13">
-      <c r="B5" s="43"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="45"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="44"/>
     </row>
     <row r="6" spans="2:13">
-      <c r="B6" s="43"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="44"/>
-      <c r="M6" s="45"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="43"/>
+      <c r="M6" s="44"/>
     </row>
     <row r="7" spans="2:13">
-      <c r="B7" s="43"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="44"/>
-      <c r="L7" s="44"/>
-      <c r="M7" s="45"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="43"/>
+      <c r="M7" s="44"/>
     </row>
     <row r="8" spans="2:13">
-      <c r="B8" s="46"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="47"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="48"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="47"/>
     </row>
     <row r="9" spans="2:13" ht="13" thickBot="1"/>
     <row r="10" spans="2:13" ht="14" thickBot="1">
@@ -1019,69 +1078,69 @@
       <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="49" t="s">
+      <c r="C11" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="49"/>
+      <c r="D11" s="48"/>
     </row>
     <row r="12" spans="2:13">
       <c r="B12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="39"/>
+      <c r="D12" s="38"/>
     </row>
     <row r="14" spans="2:13">
       <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="50" t="s">
+      <c r="C14" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
     </row>
     <row r="15" spans="2:13">
       <c r="B15" s="6">
         <v>1100859</v>
       </c>
-      <c r="C15" s="39" t="s">
+      <c r="C15" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
     </row>
     <row r="16" spans="2:13">
       <c r="B16" s="6">
         <v>1110119</v>
       </c>
-      <c r="C16" s="39" t="s">
+      <c r="C16" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
     </row>
     <row r="17" spans="2:13">
       <c r="B17" s="6">
         <v>1111168</v>
       </c>
-      <c r="C17" s="39" t="s">
+      <c r="C17" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
     </row>
     <row r="18" spans="2:13">
       <c r="B18" s="6">
         <v>1110333</v>
       </c>
-      <c r="C18" s="39" t="s">
+      <c r="C18" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
     </row>
     <row r="19" spans="2:13">
       <c r="B19" s="29"/>
@@ -1134,15 +1193,15 @@
       <c r="F25" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="G25" s="51" t="s">
+      <c r="G25" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="H25" s="52"/>
-      <c r="I25" s="52"/>
-      <c r="J25" s="52"/>
-      <c r="K25" s="52"/>
-      <c r="L25" s="52"/>
-      <c r="M25" s="53"/>
+      <c r="H25" s="51"/>
+      <c r="I25" s="51"/>
+      <c r="J25" s="51"/>
+      <c r="K25" s="51"/>
+      <c r="L25" s="51"/>
+      <c r="M25" s="52"/>
     </row>
     <row r="26" spans="2:13">
       <c r="B26" s="8">
@@ -1160,13 +1219,13 @@
       <c r="F26" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G26" s="36"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="37"/>
-      <c r="J26" s="37"/>
-      <c r="K26" s="37"/>
-      <c r="L26" s="37"/>
-      <c r="M26" s="38"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="36"/>
+      <c r="M26" s="37"/>
     </row>
     <row r="27" spans="2:13">
       <c r="B27" s="8">
@@ -1184,15 +1243,15 @@
       <c r="F27" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G27" s="36" t="s">
+      <c r="G27" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
-      <c r="K27" s="37"/>
-      <c r="L27" s="37"/>
-      <c r="M27" s="38"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="36"/>
+      <c r="M27" s="37"/>
     </row>
     <row r="28" spans="2:13">
       <c r="B28" s="8">
@@ -1210,15 +1269,15 @@
       <c r="F28" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G28" s="36" t="s">
+      <c r="G28" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
-      <c r="K28" s="37"/>
-      <c r="L28" s="37"/>
-      <c r="M28" s="38"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
+      <c r="K28" s="36"/>
+      <c r="L28" s="36"/>
+      <c r="M28" s="37"/>
     </row>
     <row r="29" spans="2:13">
       <c r="B29" s="12">
@@ -1236,15 +1295,15 @@
       <c r="F29" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G29" s="36" t="s">
+      <c r="G29" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
-      <c r="K29" s="37"/>
-      <c r="L29" s="37"/>
-      <c r="M29" s="38"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="36"/>
+      <c r="J29" s="36"/>
+      <c r="K29" s="36"/>
+      <c r="L29" s="36"/>
+      <c r="M29" s="37"/>
     </row>
     <row r="30" spans="2:13">
       <c r="B30" s="17"/>
@@ -1279,7 +1338,7 @@
       <c r="C32" s="14"/>
       <c r="D32" s="14"/>
       <c r="E32" s="10"/>
-      <c r="F32" s="32" t="s">
+      <c r="F32" s="31" t="s">
         <v>20</v>
       </c>
       <c r="G32" s="26"/>
@@ -1295,7 +1354,7 @@
       <c r="C33" s="14"/>
       <c r="D33" s="14"/>
       <c r="E33" s="10"/>
-      <c r="F33" s="32" t="s">
+      <c r="F33" s="31" t="s">
         <v>21</v>
       </c>
       <c r="G33" s="26"/>
@@ -1311,7 +1370,7 @@
       <c r="C34" s="14"/>
       <c r="D34" s="14"/>
       <c r="E34" s="10"/>
-      <c r="F34" s="32" t="s">
+      <c r="F34" s="31" t="s">
         <v>24</v>
       </c>
       <c r="G34" s="26"/>
@@ -1364,7 +1423,7 @@
       <selection activeCell="L26" sqref="L26:M26"/>
       <selection pane="topRight" activeCell="L26" sqref="L26:M26"/>
       <selection pane="bottomLeft" activeCell="L26" sqref="L26:M26"/>
-      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1401,27 +1460,31 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="21"/>
-      <c r="B3" s="34">
+      <c r="B3" s="33">
         <v>1</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="34" t="s">
+      <c r="D3" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="33" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="21"/>
-      <c r="B4" s="34">
+      <c r="B4" s="33">
         <v>2</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="34" t="s">
+      <c r="D4" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="33" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1430,11 +1493,13 @@
       <c r="B5" s="22">
         <v>3</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="34" t="s">
+      <c r="D5" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="33" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1443,11 +1508,13 @@
       <c r="B6" s="22">
         <v>4</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="31"/>
-      <c r="E6" s="34" t="s">
+      <c r="D6" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="33" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1456,10 +1523,12 @@
       <c r="B7" s="22">
         <v>5</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="23"/>
+      <c r="D7" s="32" t="s">
+        <v>24</v>
+      </c>
       <c r="E7" s="23" t="s">
         <v>35</v>
       </c>
@@ -1469,10 +1538,12 @@
       <c r="B8" s="22">
         <v>6</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="23"/>
+      <c r="D8" s="32" t="s">
+        <v>24</v>
+      </c>
       <c r="E8" s="23" t="s">
         <v>35</v>
       </c>
@@ -1482,10 +1553,12 @@
       <c r="B9" s="22">
         <v>7</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="23"/>
+      <c r="D9" s="32" t="s">
+        <v>24</v>
+      </c>
       <c r="E9" s="23" t="s">
         <v>35</v>
       </c>
@@ -1495,10 +1568,12 @@
       <c r="B10" s="22">
         <v>8</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="23"/>
+      <c r="D10" s="32" t="s">
+        <v>24</v>
+      </c>
       <c r="E10" s="23" t="s">
         <v>35</v>
       </c>
@@ -1508,97 +1583,195 @@
       <c r="B11" s="22">
         <v>9</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="23"/>
+      <c r="D11" s="32" t="s">
+        <v>24</v>
+      </c>
       <c r="E11" s="23" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="21"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
+      <c r="B12" s="22">
+        <v>10</v>
+      </c>
+      <c r="C12" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="21"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
+      <c r="B13" s="22">
+        <v>11</v>
+      </c>
+      <c r="C13" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="21"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
+      <c r="B14" s="22">
+        <v>12</v>
+      </c>
+      <c r="C14" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="21"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
+      <c r="B15" s="22">
+        <v>13</v>
+      </c>
+      <c r="C15" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="21"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
+      <c r="B16" s="22">
+        <v>14</v>
+      </c>
+      <c r="C16" s="53" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="21"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
+      <c r="B17" s="22">
+        <v>15</v>
+      </c>
+      <c r="C17" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="21"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
+      <c r="B18" s="22">
+        <v>16</v>
+      </c>
+      <c r="C18" s="53" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="21"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
+      <c r="B19" s="22">
+        <v>17</v>
+      </c>
+      <c r="C19" s="53" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="21"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
+      <c r="B20" s="22">
+        <v>18</v>
+      </c>
+      <c r="C20" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="21"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
+      <c r="B21" s="22">
+        <v>19</v>
+      </c>
+      <c r="C21" s="53" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="21"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
+      <c r="B22" s="22">
+        <v>20</v>
+      </c>
+      <c r="C22" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="21"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
+      <c r="B23" s="22">
+        <v>21</v>
+      </c>
+      <c r="C23" s="53" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="21"/>
@@ -1679,11 +1852,12 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D24:D33">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Finished final scrum document
</commit_message>
<xml_diff>
--- a/Documentation/Sprint Planning/Planning - NaaiTek.xlsx
+++ b/Documentation/Sprint Planning/Planning - NaaiTek.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Documents\LAPR5\Documentation\Sprint Planning\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14700" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Description and Releases" sheetId="1" r:id="rId1"/>
@@ -50,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="102">
   <si>
     <t>ISSUE</t>
   </si>
@@ -224,6 +229,138 @@
   </si>
   <si>
     <t>JC</t>
+  </si>
+  <si>
+    <t>Create TAGs</t>
+  </si>
+  <si>
+    <t>Service returning user's graph</t>
+  </si>
+  <si>
+    <t>Connect C++ to Database</t>
+  </si>
+  <si>
+    <t>Tic-Tac-Toe Logic</t>
+  </si>
+  <si>
+    <t>Hangman Logic</t>
+  </si>
+  <si>
+    <t>Labyrinth Logic</t>
+  </si>
+  <si>
+    <t>Suggest Connection</t>
+  </si>
+  <si>
+    <t>Add and remove friends</t>
+  </si>
+  <si>
+    <t>Network dimension (all users)</t>
+  </si>
+  <si>
+    <t>Network dimensions (for authenticated user)</t>
+  </si>
+  <si>
+    <t>Leaderboards</t>
+  </si>
+  <si>
+    <t>Tag Cloud (All users)</t>
+  </si>
+  <si>
+    <t>Tag Cloud (users)</t>
+  </si>
+  <si>
+    <t>Friend Suggestion</t>
+  </si>
+  <si>
+    <t>Edit connections between users</t>
+  </si>
+  <si>
+    <t>User authentication window (visual c++)</t>
+  </si>
+  <si>
+    <t>Add friend</t>
+  </si>
+  <si>
+    <t>Remove friend</t>
+  </si>
+  <si>
+    <t>Check HTTP access</t>
+  </si>
+  <si>
+    <t>Check all active webservices</t>
+  </si>
+  <si>
+    <t>Check free disk space</t>
+  </si>
+  <si>
+    <t>Check CPU usage</t>
+  </si>
+  <si>
+    <t>Check network interface usage</t>
+  </si>
+  <si>
+    <t>Check number of registered users</t>
+  </si>
+  <si>
+    <t>Check download tax</t>
+  </si>
+  <si>
+    <t>Unresolved</t>
+  </si>
+  <si>
+    <t>Nodes and paths visual improvement</t>
+  </si>
+  <si>
+    <t>Overall graphical improvements</t>
+  </si>
+  <si>
+    <t>Associate mini-games</t>
+  </si>
+  <si>
+    <t>Connect c++ to prolog ws</t>
+  </si>
+  <si>
+    <t>Game Modes</t>
+  </si>
+  <si>
+    <t>Add sound to the game</t>
+  </si>
+  <si>
+    <t>Show the common friends with another friend in another graph</t>
+  </si>
+  <si>
+    <t>Create a graph with common friends between two users</t>
+  </si>
+  <si>
+    <t>Send friend requests in-game</t>
+  </si>
+  <si>
+    <t>Show the shortest and the strongest path between two users</t>
+  </si>
+  <si>
+    <t>List the network strenght for each user</t>
+  </si>
+  <si>
+    <t>Read notifications</t>
+  </si>
+  <si>
+    <t>Add words for Hangman minigame on the website</t>
+  </si>
+  <si>
+    <t>Show user names</t>
+  </si>
+  <si>
+    <t>Implement external menus</t>
+  </si>
+  <si>
+    <t>friend Suggestion</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Viewport for user notification</t>
+  </si>
+  <si>
+    <t>Invalid</t>
   </si>
 </sst>
 </file>
@@ -233,7 +370,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yy;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -270,6 +407,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -504,7 +647,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -547,9 +690,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -574,6 +714,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -629,16 +775,28 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -943,19 +1101,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M35"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="S31" sqref="S31"/>
+    <sheetView topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.1640625" customWidth="1"/>
-    <col min="2" max="2" width="10.5" customWidth="1"/>
-    <col min="6" max="6" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="13" thickBot="1"/>
-    <row r="2" spans="2:13" ht="14" thickBot="1">
+    <row r="1" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
@@ -971,94 +1129,94 @@
       <c r="L2" s="2"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="2:13">
-      <c r="B3" s="39" t="s">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B3" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="41"/>
-    </row>
-    <row r="4" spans="2:13">
-      <c r="B4" s="42"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
-      <c r="M4" s="44"/>
-    </row>
-    <row r="5" spans="2:13">
-      <c r="B5" s="42"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="43"/>
-      <c r="M5" s="44"/>
-    </row>
-    <row r="6" spans="2:13">
-      <c r="B6" s="42"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
-      <c r="L6" s="43"/>
-      <c r="M6" s="44"/>
-    </row>
-    <row r="7" spans="2:13">
-      <c r="B7" s="42"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="43"/>
-      <c r="M7" s="44"/>
-    </row>
-    <row r="8" spans="2:13">
-      <c r="B8" s="45"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="46"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="46"/>
-      <c r="M8" s="47"/>
-    </row>
-    <row r="9" spans="2:13" ht="13" thickBot="1"/>
-    <row r="10" spans="2:13" ht="14" thickBot="1">
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="42"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B4" s="43"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="45"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B5" s="43"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="45"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B6" s="43"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="45"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B7" s="43"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="44"/>
+      <c r="M7" s="45"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B8" s="46"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="48"/>
+    </row>
+    <row r="9" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1074,94 +1232,94 @@
       <c r="L10" s="2"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="2:13">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="48"/>
-    </row>
-    <row r="12" spans="2:13">
+      <c r="D11" s="49"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="38"/>
-    </row>
-    <row r="14" spans="2:13">
+      <c r="D12" s="39"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="49" t="s">
+      <c r="C14" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-    </row>
-    <row r="15" spans="2:13">
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B15" s="6">
         <v>1100859</v>
       </c>
-      <c r="C15" s="38" t="s">
+      <c r="C15" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-    </row>
-    <row r="16" spans="2:13">
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B16" s="6">
         <v>1110119</v>
       </c>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-    </row>
-    <row r="17" spans="2:13">
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B17" s="6">
         <v>1111168</v>
       </c>
-      <c r="C17" s="38" t="s">
+      <c r="C17" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-    </row>
-    <row r="18" spans="2:13">
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B18" s="6">
         <v>1110333</v>
       </c>
-      <c r="C18" s="38" t="s">
+      <c r="C18" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-    </row>
-    <row r="19" spans="2:13">
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-    </row>
-    <row r="20" spans="2:13">
-      <c r="B20" s="30"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-    </row>
-    <row r="21" spans="2:13">
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-    </row>
-    <row r="22" spans="2:13" ht="13" thickBot="1"/>
-    <row r="23" spans="2:13" ht="14" thickBot="1">
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+    </row>
+    <row r="22" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
         <v>14</v>
       </c>
@@ -1177,7 +1335,7 @@
       <c r="L23" s="2"/>
       <c r="M23" s="3"/>
     </row>
-    <row r="25" spans="2:13" ht="25.5" customHeight="1">
+    <row r="25" spans="2:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="7" t="s">
         <v>15</v>
       </c>
@@ -1190,20 +1348,20 @@
       <c r="E25" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F25" s="27" t="s">
+      <c r="F25" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="G25" s="50" t="s">
+      <c r="G25" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="H25" s="51"/>
-      <c r="I25" s="51"/>
-      <c r="J25" s="51"/>
-      <c r="K25" s="51"/>
-      <c r="L25" s="51"/>
-      <c r="M25" s="52"/>
-    </row>
-    <row r="26" spans="2:13">
+      <c r="H25" s="52"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="52"/>
+      <c r="K25" s="52"/>
+      <c r="L25" s="52"/>
+      <c r="M25" s="53"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B26" s="8">
         <v>1</v>
       </c>
@@ -1217,17 +1375,17 @@
         <v>5</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G26" s="35"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="36"/>
-      <c r="K26" s="36"/>
-      <c r="L26" s="36"/>
-      <c r="M26" s="37"/>
-    </row>
-    <row r="27" spans="2:13">
+        <v>24</v>
+      </c>
+      <c r="G26" s="36"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37"/>
+      <c r="M26" s="38"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B27" s="8">
         <v>2</v>
       </c>
@@ -1241,19 +1399,19 @@
         <v>7</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G27" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="G27" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
-      <c r="K27" s="36"/>
-      <c r="L27" s="36"/>
-      <c r="M27" s="37"/>
-    </row>
-    <row r="28" spans="2:13">
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="37"/>
+      <c r="L27" s="37"/>
+      <c r="M27" s="38"/>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B28" s="8">
         <v>3</v>
       </c>
@@ -1267,19 +1425,19 @@
         <v>8</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G28" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="G28" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
-      <c r="K28" s="36"/>
-      <c r="L28" s="36"/>
-      <c r="M28" s="37"/>
-    </row>
-    <row r="29" spans="2:13">
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
+      <c r="K28" s="37"/>
+      <c r="L28" s="37"/>
+      <c r="M28" s="38"/>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B29" s="12">
         <v>4</v>
       </c>
@@ -1293,95 +1451,95 @@
         <v>7</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G29" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="G29" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="H29" s="36"/>
-      <c r="I29" s="36"/>
-      <c r="J29" s="36"/>
-      <c r="K29" s="36"/>
-      <c r="L29" s="36"/>
-      <c r="M29" s="37"/>
-    </row>
-    <row r="30" spans="2:13">
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
+      <c r="K29" s="37"/>
+      <c r="L29" s="37"/>
+      <c r="M29" s="38"/>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B30" s="17"/>
       <c r="C30" s="15"/>
       <c r="D30" s="15"/>
       <c r="E30" s="16"/>
       <c r="F30" s="16"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="25"/>
-      <c r="I30" s="25"/>
-      <c r="J30" s="25"/>
-      <c r="K30" s="25"/>
-      <c r="L30" s="25"/>
-      <c r="M30" s="25"/>
-    </row>
-    <row r="31" spans="2:13">
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="24"/>
+      <c r="L30" s="24"/>
+      <c r="M30" s="24"/>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B31" s="18"/>
       <c r="C31" s="14"/>
       <c r="D31" s="14"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="26"/>
-      <c r="K31" s="26"/>
-      <c r="L31" s="26"/>
-      <c r="M31" s="26"/>
-    </row>
-    <row r="32" spans="2:13">
+      <c r="G31" s="25"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="25"/>
+      <c r="J31" s="25"/>
+      <c r="K31" s="25"/>
+      <c r="L31" s="25"/>
+      <c r="M31" s="25"/>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B32" s="18"/>
       <c r="C32" s="14"/>
       <c r="D32" s="14"/>
       <c r="E32" s="10"/>
-      <c r="F32" s="31" t="s">
+      <c r="F32" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="G32" s="26"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="26"/>
-      <c r="K32" s="26"/>
-      <c r="L32" s="26"/>
-      <c r="M32" s="26"/>
-    </row>
-    <row r="33" spans="2:13">
+      <c r="G32" s="25"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="25"/>
+      <c r="K32" s="25"/>
+      <c r="L32" s="25"/>
+      <c r="M32" s="25"/>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B33" s="18"/>
       <c r="C33" s="14"/>
       <c r="D33" s="14"/>
       <c r="E33" s="10"/>
-      <c r="F33" s="31" t="s">
+      <c r="F33" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="G33" s="26"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="26"/>
-      <c r="J33" s="26"/>
-      <c r="K33" s="26"/>
-      <c r="L33" s="26"/>
-      <c r="M33" s="26"/>
-    </row>
-    <row r="34" spans="2:13">
+      <c r="G33" s="25"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="25"/>
+      <c r="L33" s="25"/>
+      <c r="M33" s="25"/>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B34" s="18"/>
       <c r="C34" s="14"/>
       <c r="D34" s="14"/>
       <c r="E34" s="10"/>
-      <c r="F34" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="26"/>
-      <c r="K34" s="26"/>
-      <c r="L34" s="26"/>
-      <c r="M34" s="26"/>
-    </row>
-    <row r="35" spans="2:13">
+      <c r="F34" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="G34" s="25"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="25"/>
+      <c r="L34" s="25"/>
+      <c r="M34" s="25"/>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B35" s="19"/>
     </row>
   </sheetData>
@@ -1416,448 +1574,967 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection activeCell="L26" sqref="L26:M26"/>
       <selection pane="topRight" activeCell="L26" sqref="L26:M26"/>
       <selection pane="bottomLeft" activeCell="L26" sqref="L26:M26"/>
-      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomRight" activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.83203125" style="20" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" style="20" customWidth="1"/>
-    <col min="3" max="3" width="44.83203125" style="20" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" style="20" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" style="20" customWidth="1"/>
-    <col min="6" max="16384" width="8.83203125" style="20"/>
+    <col min="1" max="1" width="3.85546875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="20" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" style="20" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="20" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" style="20" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="21"/>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
       <c r="E1" s="21"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="21"/>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="21"/>
-      <c r="B3" s="33">
+      <c r="B3" s="32">
         <v>1</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="33" t="s">
+      <c r="D3" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="32" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="21"/>
-      <c r="B4" s="33">
+      <c r="B4" s="32">
         <v>2</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="33" t="s">
+      <c r="D4" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="32" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14.25" customHeight="1">
+    <row r="5" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="21"/>
       <c r="B5" s="22">
         <v>3</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="33" t="s">
+      <c r="D5" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="32" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14.25" customHeight="1">
+    <row r="6" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="21"/>
       <c r="B6" s="22">
         <v>4</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="33" t="s">
+      <c r="D6" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="32" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="21"/>
       <c r="B7" s="22">
         <v>5</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="31" t="s">
         <v>24</v>
       </c>
       <c r="E7" s="23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="21"/>
       <c r="B8" s="22">
         <v>6</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="31" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="13.5" customHeight="1">
+    <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="21"/>
       <c r="B9" s="22">
         <v>7</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="32" t="s">
+      <c r="D9" s="31" t="s">
         <v>24</v>
       </c>
       <c r="E9" s="23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="21"/>
       <c r="B10" s="22">
         <v>8</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="31" t="s">
         <v>24</v>
       </c>
       <c r="E10" s="23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="21"/>
       <c r="B11" s="22">
         <v>9</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="31" t="s">
         <v>24</v>
       </c>
       <c r="E11" s="23" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="21"/>
       <c r="B12" s="22">
         <v>10</v>
       </c>
-      <c r="C12" s="53" t="s">
+      <c r="C12" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="31" t="s">
         <v>24</v>
       </c>
       <c r="E12" s="23" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="21"/>
       <c r="B13" s="22">
         <v>11</v>
       </c>
-      <c r="C13" s="53" t="s">
+      <c r="C13" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="32" t="s">
-        <v>21</v>
+      <c r="D13" s="31" t="s">
+        <v>24</v>
       </c>
       <c r="E13" s="23" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="21"/>
       <c r="B14" s="22">
         <v>12</v>
       </c>
-      <c r="C14" s="53" t="s">
+      <c r="C14" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="32" t="s">
-        <v>21</v>
+      <c r="D14" s="31" t="s">
+        <v>24</v>
       </c>
       <c r="E14" s="23" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="21"/>
       <c r="B15" s="22">
         <v>13</v>
       </c>
-      <c r="C15" s="53" t="s">
+      <c r="C15" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="32" t="s">
-        <v>21</v>
+      <c r="D15" s="31" t="s">
+        <v>24</v>
       </c>
       <c r="E15" s="23" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="21"/>
       <c r="B16" s="22">
         <v>14</v>
       </c>
-      <c r="C16" s="53" t="s">
+      <c r="C16" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="32" t="s">
-        <v>21</v>
+      <c r="D16" s="31" t="s">
+        <v>24</v>
       </c>
       <c r="E16" s="23" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="21"/>
       <c r="B17" s="22">
         <v>15</v>
       </c>
-      <c r="C17" s="53" t="s">
+      <c r="C17" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="32" t="s">
-        <v>21</v>
+      <c r="D17" s="31" t="s">
+        <v>24</v>
       </c>
       <c r="E17" s="23" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="21"/>
       <c r="B18" s="22">
         <v>16</v>
       </c>
-      <c r="C18" s="53" t="s">
+      <c r="C18" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="32" t="s">
-        <v>21</v>
+      <c r="D18" s="31" t="s">
+        <v>24</v>
       </c>
       <c r="E18" s="23" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="21"/>
       <c r="B19" s="22">
         <v>17</v>
       </c>
-      <c r="C19" s="53" t="s">
+      <c r="C19" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="32" t="s">
-        <v>21</v>
+      <c r="D19" s="31" t="s">
+        <v>24</v>
       </c>
       <c r="E19" s="23" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="21"/>
       <c r="B20" s="22">
         <v>18</v>
       </c>
-      <c r="C20" s="53" t="s">
+      <c r="C20" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="32" t="s">
-        <v>21</v>
+      <c r="D20" s="31" t="s">
+        <v>24</v>
       </c>
       <c r="E20" s="23" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="21"/>
       <c r="B21" s="22">
         <v>19</v>
       </c>
-      <c r="C21" s="53" t="s">
+      <c r="C21" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="32" t="s">
-        <v>21</v>
+      <c r="D21" s="31" t="s">
+        <v>24</v>
       </c>
       <c r="E21" s="23" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="21"/>
       <c r="B22" s="22">
         <v>20</v>
       </c>
-      <c r="C22" s="53" t="s">
+      <c r="C22" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="32" t="s">
-        <v>21</v>
+      <c r="D22" s="31" t="s">
+        <v>24</v>
       </c>
       <c r="E22" s="23" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="21"/>
       <c r="B23" s="22">
         <v>21</v>
       </c>
-      <c r="C23" s="53" t="s">
+      <c r="C23" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="32" t="s">
-        <v>21</v>
+      <c r="D23" s="31" t="s">
+        <v>24</v>
       </c>
       <c r="E23" s="23" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="21"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="B24" s="22">
+        <v>22</v>
+      </c>
+      <c r="C24" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="21"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="B25" s="22">
+        <v>23</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="21"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="B26" s="22">
+        <v>24</v>
+      </c>
+      <c r="C26" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="21"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="B27" s="22">
+        <v>25</v>
+      </c>
+      <c r="C27" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="21"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="B28" s="22">
+        <v>26</v>
+      </c>
+      <c r="C28" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" s="23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="21"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="B29" s="22">
+        <v>27</v>
+      </c>
+      <c r="C29" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="21"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="B30" s="22">
+        <v>28</v>
+      </c>
+      <c r="C30" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="21"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
+      <c r="B31" s="22">
+        <v>29</v>
+      </c>
+      <c r="C31" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" s="56" t="s">
+        <v>101</v>
+      </c>
       <c r="E31" s="23"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="21"/>
-      <c r="B32" s="22"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="B32" s="22">
+        <v>30</v>
+      </c>
+      <c r="C32" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" s="23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="21"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="B33" s="22">
+        <v>31</v>
+      </c>
+      <c r="C33" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E33" s="23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="21"/>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
+      <c r="B34" s="22">
+        <v>32</v>
+      </c>
+      <c r="C34" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E34" s="54" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B35" s="22">
+        <v>33</v>
+      </c>
+      <c r="C35" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E35" s="55" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="22">
+        <v>34</v>
+      </c>
+      <c r="C36" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="D36" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" s="55" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B37" s="22">
+        <v>35</v>
+      </c>
+      <c r="C37" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E37" s="55" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B38" s="22">
+        <v>36</v>
+      </c>
+      <c r="C38" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="D38" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E38" s="55" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B39" s="22">
+        <v>37</v>
+      </c>
+      <c r="C39" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="D39" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E39" s="55" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B40" s="22">
+        <v>38</v>
+      </c>
+      <c r="C40" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="D40" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E40" s="55" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B41" s="22">
+        <v>39</v>
+      </c>
+      <c r="C41" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="D41" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E41" s="55" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B42" s="22">
+        <v>40</v>
+      </c>
+      <c r="C42" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="D42" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E42" s="55" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B43" s="22">
+        <v>41</v>
+      </c>
+      <c r="C43" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="D43" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E43" s="55" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B44" s="22">
+        <v>42</v>
+      </c>
+      <c r="C44" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="D44" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" s="55" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B45" s="22">
+        <v>43</v>
+      </c>
+      <c r="C45" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="D45" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E45" s="55" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B46" s="22">
+        <v>44</v>
+      </c>
+      <c r="C46" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="D46" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E46" s="55" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B47" s="22">
+        <v>45</v>
+      </c>
+      <c r="C47" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="D47" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E47" s="55" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B48" s="22">
+        <v>46</v>
+      </c>
+      <c r="C48" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="D48" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="E48" s="55" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B49" s="22">
+        <v>47</v>
+      </c>
+      <c r="C49" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="D49" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E49" s="55" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B50" s="22">
+        <v>48</v>
+      </c>
+      <c r="C50" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="D50" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E50" s="55" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B51" s="22">
+        <v>49</v>
+      </c>
+      <c r="C51" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="D51" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E51" s="55" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B52" s="22">
+        <v>50</v>
+      </c>
+      <c r="C52" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="D52" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E52" s="55" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B53" s="22">
+        <v>51</v>
+      </c>
+      <c r="C53" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="D53" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="E53" s="55"/>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B54" s="22">
+        <v>52</v>
+      </c>
+      <c r="C54" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="D54" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E54" s="55" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B55" s="22">
+        <v>53</v>
+      </c>
+      <c r="C55" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="D55" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E55" s="55" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B56" s="22">
+        <v>54</v>
+      </c>
+      <c r="C56" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="D56" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E56" s="55" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B57" s="22">
+        <v>55</v>
+      </c>
+      <c r="C57" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="D57" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E57" s="55" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B58" s="22">
+        <v>56</v>
+      </c>
+      <c r="C58" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="D58" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E58" s="55" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B59" s="22">
+        <v>57</v>
+      </c>
+      <c r="C59" s="58" t="s">
+        <v>99</v>
+      </c>
+      <c r="D59" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E59" s="55" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B60" s="22">
+        <v>58</v>
+      </c>
+      <c r="C60" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="D60" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E60" s="55" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B61" s="22">
+        <v>59</v>
+      </c>
+      <c r="C61" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="D61" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E61" s="55" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B62" s="22">
+        <v>60</v>
+      </c>
+      <c r="C62" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="D62" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E62" s="55" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B63" s="22">
+        <v>61</v>
+      </c>
+      <c r="C63" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="D63" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E63" s="55" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B64" s="22">
+        <v>62</v>
+      </c>
+      <c r="C64" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="D64" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E64" s="55" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B65" s="22">
+        <v>63</v>
+      </c>
+      <c r="C65" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="D65" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E65" s="55" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B66" s="22"/>
+      <c r="C66" s="55"/>
+      <c r="D66" s="32"/>
+      <c r="E66" s="55"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D24:D33">
-      <formula1>#REF!</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>